<commit_message>
Updates, working UVM bring-up environment
</commit_message>
<xml_diff>
--- a/Problems_and_Solutions.xlsx
+++ b/Problems_and_Solutions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Graduation Project\Siemens\DP_Verification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{475E8565-8A0E-4023-BA43-E6A9D51E2BA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5117A7F3-6282-4341-AAE6-363EC3FD1B18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{439A0188-48B4-4D9A-A1AE-90D8E4E83E19}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Problems</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>A fatal issue arised due to the objections in the test class.</t>
+  </si>
+  <si>
+    <t>due to a coding mistake of writing phase inside raise.objection()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">write this in raise.objection() </t>
   </si>
 </sst>
 </file>
@@ -92,7 +98,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -102,6 +108,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -440,7 +452,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -472,9 +484,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>